<commit_message>
The final module added outputs the combined expenses as a sheet and the percentages as a sheet
</commit_message>
<xml_diff>
--- a/Practice3/Percentage of Expenses.xlsx
+++ b/Practice3/Percentage of Expenses.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dkmk1\OneDrive\Documents\UiPath\Lesson3\Practice3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9556BEE9-E762-4EA5-9F7B-586B6FEBE756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F3BD40-CD9C-441F-AC53-9ED73C2E5C74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21520" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15585" yWindow="-13620" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Percentage of Expenses" sheetId="4" r:id="rId1"/>
+    <sheet name="Combined Expenses" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="26">
   <si>
     <t>Gym membership</t>
   </si>
@@ -58,6 +59,51 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Vacation</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>Rent</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Plumbing</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>01.01.2019</t>
+  </si>
+  <si>
+    <t>07.01.2019</t>
+  </si>
+  <si>
+    <t>01.02.2019</t>
+  </si>
+  <si>
+    <t>01.03.2019</t>
+  </si>
+  <si>
+    <t>01.04.2019</t>
+  </si>
+  <si>
+    <t>01.05.2019</t>
+  </si>
+  <si>
+    <t>Expense Type</t>
+  </si>
+  <si>
+    <t>Expense Percentage</t>
   </si>
 </sst>
 </file>
@@ -95,7 +141,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,67 +421,521 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6220DE62-920D-4E8B-B43E-020627CE4A5C}">
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="A1:D7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.24970000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>9.64E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.1206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.36170000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2.6599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2.18E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.7100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>6.1899999999999997E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2.0500000000000001E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FAA90B-0588-4055-84CF-7FE8B578B7D0}">
+  <dimension ref="A1:C36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B33" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C33">
         <v>452</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B34" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C34">
         <v>354</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B35" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C35">
         <v>1283</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B36" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C36">
         <v>425</v>
       </c>
     </row>

</xml_diff>